<commit_message>
Mantenimiento de Tipo de Suplidor
</commit_message>
<xml_diff>
--- a/Puntos Pendientes.xlsx
+++ b/Puntos Pendientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ing.Juan Marcelino\Documents\Desarrollo de Software\Jdiaz0624\DSMarket.Solucion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316640D7-9B3C-48BF-92F3-687FCCD76645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED035494-8353-4E22-A8D9-1764BB4EEB7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B417D3C8-BE99-423E-9CA8-BAFE0CA7DDA1}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2"/>

</xml_diff>

<commit_message>
Cambio en Facturas Minimizadas
</commit_message>
<xml_diff>
--- a/Puntos Pendientes.xlsx
+++ b/Puntos Pendientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ing.Juan Marcelino\Source\Repos\Jdiaz0624\DSMarket.Solucion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSP-D-024\source\repos\Jdiaz0624\DSMarket.Solucion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324C25AA-237E-4495-A8F0-20CEDB4F3C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B9EDE2-628F-444E-8E2A-8D94F5865DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B417D3C8-BE99-423E-9CA8-BAFE0CA7DDA1}"/>
+    <workbookView xWindow="-28920" yWindow="-1755" windowWidth="29040" windowHeight="15840" xr2:uid="{B417D3C8-BE99-423E-9CA8-BAFE0CA7DDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Servicio</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Generar Backup BD</t>
   </si>
   <si>
-    <t>Realizar Ventas a Creditos</t>
-  </si>
-  <si>
     <t>Reportes</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Reporte de Ganancia de Venta</t>
   </si>
   <si>
-    <t>Antiguedad de Saldo</t>
-  </si>
-  <si>
     <t>Reporte 606</t>
   </si>
   <si>
@@ -192,52 +186,16 @@
     <t>Mantenimiento de Compras</t>
   </si>
   <si>
-    <t>Contabilidad</t>
-  </si>
-  <si>
-    <t>Control de Apertura</t>
-  </si>
-  <si>
-    <t>Catalogo de Cuenta</t>
-  </si>
-  <si>
-    <t>Impresion de cheques</t>
-  </si>
-  <si>
-    <t>Movimientos</t>
-  </si>
-  <si>
-    <t>Movimientos Fijos</t>
-  </si>
-  <si>
     <t>Procesar Productos Defectuosos</t>
   </si>
   <si>
-    <t>CXC</t>
-  </si>
-  <si>
-    <t>CXP</t>
-  </si>
-  <si>
-    <t>Balance General</t>
-  </si>
-  <si>
     <t>Estado de Resultado</t>
   </si>
   <si>
-    <t>Libro Mayor</t>
-  </si>
-  <si>
-    <t>Estado de Flujo mayor de efectivo</t>
-  </si>
-  <si>
-    <t>Reporte de Impuestos y Retenciones</t>
-  </si>
-  <si>
     <t>Imprimir Factura a Punto de Venta</t>
   </si>
   <si>
-    <t>D</t>
+    <t>Reporte de Estado de Situacion</t>
   </si>
 </sst>
 </file>
@@ -353,9 +311,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,10 +631,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,11 +646,10 @@
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -711,13 +668,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -737,13 +691,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -763,13 +714,10 @@
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -784,16 +732,13 @@
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -805,19 +750,16 @@
         <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -825,21 +767,18 @@
         <v>12</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>52</v>
+      <c r="D6" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -848,22 +787,19 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
+      <c r="G7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
@@ -871,114 +807,90 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="G13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="7" t="s">
-        <v>65</v>
+      <c r="G17" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="G18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>